<commit_message>
Updated .xlsx template to match code changes
</commit_message>
<xml_diff>
--- a/c-gen/Template.xlsx
+++ b/c-gen/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reacher-nrfc\reach_code_generator_util\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-silabs\reach-util\c-gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB44B33-818F-4733-8AD7-715E726E6DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D429EB-662E-49AD-96C8-E5A06690AFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10090" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1944" yWindow="840" windowWidth="19176" windowHeight="10296" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <sheet name="Example Bitfield" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Device Name</t>
   </si>
@@ -89,12 +90,15 @@
   <si>
     <t>No</t>
   </si>
+  <si>
+    <t>Require Checksum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +129,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -155,6 +167,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,8 +389,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2402,10 +2415,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D998"/>
+  <dimension ref="A1:E998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2426,7 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2426,91 +2439,94 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -7426,7 +7442,7 @@
       <c r="D998" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{B4A9057C-0490-4C7A-AD27-4B4DDBCECFFF}">
       <formula1>"None,Read,Write,Read/Write"</formula1>
     </dataValidation>
@@ -7442,8 +7458,12 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid File Size" error="Files must have a size greater than 0 bytes" sqref="B2" xr:uid="{819C5AC3-88BA-4FE6-94AF-836E0B15B76D}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{C7CAA0AF-09A1-43C8-B3D9-2DB4DE0C58B5}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Generate max file size.  Updated template.  Scans notification stuff, but doesn't write it yet.
</commit_message>
<xml_diff>
--- a/c-gen/Template.xlsx
+++ b/c-gen/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-silabs\reach-util\c-gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\reach-util\c-gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D429EB-662E-49AD-96C8-E5A06690AFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E109F1A-C006-4EAC-84F5-2126F3F8304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1944" yWindow="840" windowWidth="19176" windowHeight="10296" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15228" yWindow="6444" windowWidth="27996" windowHeight="18600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,11 @@
     <sheet name="Example Bitfield" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Device Name</t>
   </si>
@@ -93,6 +92,21 @@
   <si>
     <t>Require Checksum</t>
   </si>
+  <si>
+    <t>Max Size</t>
+  </si>
+  <si>
+    <t>Notify</t>
+  </si>
+  <si>
+    <t>min period</t>
+  </si>
+  <si>
+    <t>max period</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
 </sst>
 </file>
 
@@ -110,12 +124,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,11 +139,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -471,7 +489,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -515,6 +533,18 @@
       <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -2415,10 +2445,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2426,7 +2456,7 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2442,91 +2472,94 @@
       <c r="E1" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>